<commit_message>
3D CAD Stage 1
Done up to Arm 1
</commit_message>
<xml_diff>
--- a/BOM & info.xlsx
+++ b/BOM & info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a909ac0df12032b6/MSc Robotics/GIC/RobotKinematics-Remote/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{81686523-6045-434A-8F1A-1DA700BE3ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{73882FDD-2482-4A7F-8C3D-8268A14EF70A}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{81686523-6045-434A-8F1A-1DA700BE3ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CDA3BF84-A4D3-4D8E-91EB-17EC01C5B9B1}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2424" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C8753E82-3F15-457C-882E-D25984A5423B}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C8753E82-3F15-457C-882E-D25984A5423B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,9 +133,6 @@
     <t>Ball Casters</t>
   </si>
   <si>
-    <t>https://shop.pimoroni.com/products/pololu-ball-caster-with-3-4-metal-ball?variant=415237741</t>
-  </si>
-  <si>
     <t>3D print</t>
   </si>
   <si>
@@ -151,7 +148,10 @@
     <t>Stepper motors FIT0503 - DFRobot</t>
   </si>
   <si>
-    <t>https://www.digikey.co.uk/product-detail/en/dfrobot/FIT0503/FIT0503-ND/7067735</t>
+    <t>https://www.dfrobot.com/product-509.html</t>
+  </si>
+  <si>
+    <t>https://www.dfrobot.com/product-1508.html</t>
   </si>
 </sst>
 </file>
@@ -178,10 +178,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -201,16 +203,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -653,12 +658,12 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -672,7 +677,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,7 +748,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -755,7 +760,7 @@
         <f t="shared" si="0"/>
         <v>10.62</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -824,8 +829,8 @@
         <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
-      <c r="F8" t="s">
-        <v>26</v>
+      <c r="F8" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -844,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -863,7 +868,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -882,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -901,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated BOM with detail drawing
</commit_message>
<xml_diff>
--- a/BOM & info.xlsx
+++ b/BOM & info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a909ac0df12032b6/MSc Robotics/GIC/RobotKinematics-Remote/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{81686523-6045-434A-8F1A-1DA700BE3ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D88E256C-FA6A-4E79-95B2-7F2E15C4E320}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{81686523-6045-434A-8F1A-1DA700BE3ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{874247D2-E5BC-4385-B241-538757524E7B}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C8753E82-3F15-457C-882E-D25984A5423B}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{C8753E82-3F15-457C-882E-D25984A5423B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -279,6 +279,67 @@
         <a:xfrm>
           <a:off x="205740" y="2307145"/>
           <a:ext cx="5554980" cy="4162233"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75C9E95D-B839-4EC8-97C8-8E84E32EF6D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="251460" y="6797040"/>
+          <a:ext cx="5951220" cy="7932420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -613,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21238CAD-6B1B-471C-8096-6749459AB4B1}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E9469C-2C3E-4DDE-A657-7645A26DA7B8}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Edited Base and Motor mount
</commit_message>
<xml_diff>
--- a/BOM & info.xlsx
+++ b/BOM & info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a909ac0df12032b6/MSc Robotics/GIC/RobotKinematics-Remote/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\MSc Robotics\GIC\RobotKinematics-Remote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{81686523-6045-434A-8F1A-1DA700BE3ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{874247D2-E5BC-4385-B241-538757524E7B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A264909-6B67-43A2-8235-BE40611A2310}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{C8753E82-3F15-457C-882E-D25984A5423B}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C8753E82-3F15-457C-882E-D25984A5423B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Check on the size</t>
+    Check on the size
+Reply:
+    get the 1/2in</t>
       </text>
     </comment>
   </commentList>
@@ -667,6 +669,9 @@
   <threadedComment ref="F8" dT="2020-12-27T22:21:16.94" personId="{E59E69DB-0CAD-4A6E-A5B6-2A6254EA60D8}" id="{18DF96CA-DCDC-4EB1-9E04-466883AD03F9}">
     <text>Check on the size</text>
   </threadedComment>
+  <threadedComment ref="F8" dT="2021-01-17T20:43:49.75" personId="{E59E69DB-0CAD-4A6E-A5B6-2A6254EA60D8}" id="{5704A47C-17FE-405A-A170-F2D5DE2CD051}" parentId="{18DF96CA-DCDC-4EB1-9E04-466883AD03F9}">
+    <text>get the 1/2in</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -674,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21238CAD-6B1B-471C-8096-6749459AB4B1}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
@@ -740,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E9469C-2C3E-4DDE-A657-7645A26DA7B8}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,8 +1006,11 @@
       <c r="D18" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{ABF0697A-34A5-40E8-9638-4C118E8829DF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
27012021 - 3D mostly done
Parts are pretty much done
Blue tack works
rotated the motor so the wires aren't sticking out
ball caster stand is longer to account for blue tack, but can shorten if need to. The ball caster comes with spacers
</commit_message>
<xml_diff>
--- a/BOM & info.xlsx
+++ b/BOM & info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\MSc Robotics\GIC\RobotKinematics-Remote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A264909-6B67-43A2-8235-BE40611A2310}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A4D513-B773-444B-A31F-DDE03E602916}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C8753E82-3F15-457C-882E-D25984A5423B}"/>
   </bookViews>
@@ -37,17 +37,61 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={18DF96CA-DCDC-4EB1-9E04-466883AD03F9}</author>
+    <author>tc={E7FB7D4C-FA99-4659-9CC0-0C919C9D5F01}</author>
+    <author>tc={17BCF766-ABB2-4350-A0A7-725336BADFCE}</author>
+    <author>tc={1869C771-C580-41CE-9D3C-793B204B87D5}</author>
+    <author>tc={58F8599A-228D-4E1E-90E9-143A66688545}</author>
+    <author>tc={22C3FD05-C2BC-4ACA-B1F4-D6737862311B}</author>
+    <author>tc={88774207-C78B-40C9-8E79-3CBBD29570AA}</author>
   </authors>
   <commentList>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{18DF96CA-DCDC-4EB1-9E04-466883AD03F9}">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{E7FB7D4C-FA99-4659-9CC0-0C919C9D5F01}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Check on the size
-Reply:
-    get the 1/2in</t>
+    Please buy 35 for 12 sets + extra</t>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="1" shapeId="0" xr:uid="{17BCF766-ABB2-4350-A0A7-725336BADFCE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Get 15 pcs of 1/2 inches, if no stock, use the next URL on the right = total 14 pcs for 12 sets + extra</t>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="2" shapeId="0" xr:uid="{1869C771-C580-41CE-9D3C-793B204B87D5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    buy 4 packs of 8 pcs at GBP 3.99 each pack
+= total 32 pcs for 12 sets + extra</t>
+      </text>
+    </comment>
+    <comment ref="F19" authorId="3" shapeId="0" xr:uid="{58F8599A-228D-4E1E-90E9-143A66688545}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    8 with the bolts, need 1 extra. Buy M3 nuts, 50pcs at GBP1.29 for 12 sets plus extra</t>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="4" shapeId="0" xr:uid="{22C3FD05-C2BC-4ACA-B1F4-D6737862311B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    buy M3 x 6 with nuts, 2x 100pcs at GBP7.42 each = 200 pcs for 12 sets + extra</t>
+      </text>
+    </comment>
+    <comment ref="F21" authorId="5" shapeId="0" xr:uid="{88774207-C78B-40C9-8E79-3CBBD29570AA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    buy 100 pcs for GBP 6.85, for 12 sets + extra</t>
       </text>
     </comment>
   </commentList>
@@ -55,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>Objective</t>
   </si>
@@ -84,9 +128,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Qty</t>
-  </si>
-  <si>
     <t>Total Cost</t>
   </si>
   <si>
@@ -135,9 +176,6 @@
     <t>3D print</t>
   </si>
   <si>
-    <t>print</t>
-  </si>
-  <si>
     <t>6. (Future) could make an end effector that holds a pen? Depending on the torque the motor can put out, might consider future addition</t>
   </si>
   <si>
@@ -157,6 +195,57 @@
   </si>
   <si>
     <t>https://www.rapidonline.com/Pololu-953-Ball-Caster-1-2-Inch-Includes-Two-Spacers-2-Screw-Sets-75-0628?clickref=52825428&amp;IncVat=1&amp;utm_source=AffWin&amp;utm_medium=Affiliate&amp;awc=1799_1610207738_31f52f4fdca15da76236c6bddf54cdd8</t>
+  </si>
+  <si>
+    <t>Bearing Holder</t>
+  </si>
+  <si>
+    <t>Motor Mount</t>
+  </si>
+  <si>
+    <t>Shaft Attachment</t>
+  </si>
+  <si>
+    <t>608ZZ Ball Bearing</t>
+  </si>
+  <si>
+    <t>print/laminate</t>
+  </si>
+  <si>
+    <t>Ball Caster mount</t>
+  </si>
+  <si>
+    <t>M3 nut</t>
+  </si>
+  <si>
+    <t>M3 x 6 Countersunk</t>
+  </si>
+  <si>
+    <t>M1.6 x 4 Countersunk</t>
+  </si>
+  <si>
+    <t>Jumper cables</t>
+  </si>
+  <si>
+    <t>PCB extensions</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/M1-6-M2-M2-5-POZI-COUNTERSUNK-MACHINE-SCREWS-A2-STAINLESS-STEEL-POSIDRIVE-BOLTS/362984625333?hash=item548391d4b5:g:N8kAAOSwE3NerWOr</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/M2-5-M3-M4-POZI-COUNTERSUNK-MACHINE-SCREWS-WITH-NUTS-ZINC-PLATED-BZP-CSK-BOLTS/183870828562?hash=item2acf8e3012:g:dYEAAOSwLUldHkh7</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/HEXAGON-FULL-NUTS-TO-FIT-METRIC-COARSE-PITCH-BOLTS-SCREWS-A2-STAINLESS-STEEL/180963079545?hash=item2a223d7579:g:AE0AAOSwqOFb0u80</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/8-Pack-608zz-Roller-Skate-Scooter-Skateboard-Wheels-Double-Shielded-Bearings-UK/363194481518?_trkparms=ispr%3D1&amp;hash=item549013fb6e:g:FuYAAOSwkK5fviHV&amp;amdata=enc%3AAQAFAAACcBaobrjLl8XobRIiIML1V4Imu%252Fn%252BzU5L90Z278x5ickkBSh1VzQSTzkTiSV5EE%252FHQWWEHJkkKpjo09ZE0lEJ3Qi5Rqj1yDG4QGk4xXb8iEh3Bi8GUzBk18wFjp1Di5JfkQ8%252Bj2t2qoQSBs2ZRxbSFmpShSUjBLTA%252FAfmC8OaERIZgkVVzAvBBFeMYW5QkBVFg74%252Fz1Ki%252FlgLJSyws4Ny4aEP%252FqjJK0ykr5qcvJ1gb4btEBstA6SgomD9szUwT4rNAjMuiHkS3VGZRd5Vpqm3GkKHhVZkNbMRFeqceIHN5mkdTUYBmdRE4KMmhy5X2QT11A5bfhtrnIYfgZrLjv89nVWzAyNY0HWmEvNmw8wh3e3%252B7DmBYZQVrepwjJpnq7fyKtCZ4LAKaVo8oLuXP%252BpStH0zZShntDlzA0ax9Br2R16KwqPofcxq5USAX6LQcvoe3YRqDPy7l0pbTpRgg7q3x%252BBOsA94r1qBoWphH28gn1bCyRAvzRUyS32Rf1KYWXPvV5VSqnkDlrA74K18W4fXmYzv5PljXkE2rdhTtIud%252FrsK7%252FIBpgVHdCQdkszAedG%252BGkiHJVzHumA63BJZroJuAXiTjOhqxXZMgGRDFB%252FOWrGr6zzms9TP8ul0sBH6SZY%252F2XT%252B%252F4%252FR%252Fz18sIX8fkqKctOZrrJXQn6CmBfHxB5z8AUupFmCOncWao9BKfshIqpZ0avzmyqNT0xwyb6sYJdIqaCqNCDCsC1DLqLE5hFn3%252Bb8PaDSrX%252Bru10n1A6pERob4Em5N9yr%252FJGJLS%252FE9zHYcWLg8U6WJeoasymbQ0Tpc4i5SPxM3kaBumKV2kH0%252Bsl9rA%253D%253D%7Ccksum%3A363194481518319458494b184b6b80b531f48d292915%7Campid%3APL_CLK%7Cclp%3A2334524</t>
+  </si>
+  <si>
+    <t>Whiteboard marker</t>
+  </si>
+  <si>
+    <t>Qty for 1 set</t>
   </si>
 </sst>
 </file>
@@ -166,7 +255,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +278,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -666,11 +761,24 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F8" dT="2020-12-27T22:21:16.94" personId="{E59E69DB-0CAD-4A6E-A5B6-2A6254EA60D8}" id="{18DF96CA-DCDC-4EB1-9E04-466883AD03F9}">
-    <text>Check on the size</text>
+  <threadedComment ref="F4" dT="2021-01-27T21:52:24.17" personId="{E59E69DB-0CAD-4A6E-A5B6-2A6254EA60D8}" id="{E7FB7D4C-FA99-4659-9CC0-0C919C9D5F01}">
+    <text>Please buy 35 for 12 sets + extra</text>
   </threadedComment>
-  <threadedComment ref="F8" dT="2021-01-17T20:43:49.75" personId="{E59E69DB-0CAD-4A6E-A5B6-2A6254EA60D8}" id="{5704A47C-17FE-405A-A170-F2D5DE2CD051}" parentId="{18DF96CA-DCDC-4EB1-9E04-466883AD03F9}">
-    <text>get the 1/2in</text>
+  <threadedComment ref="F8" dT="2021-01-27T21:45:59.50" personId="{E59E69DB-0CAD-4A6E-A5B6-2A6254EA60D8}" id="{17BCF766-ABB2-4350-A0A7-725336BADFCE}">
+    <text>Get 15 pcs of 1/2 inches, if no stock, use the next URL on the right = total 14 pcs for 12 sets + extra</text>
+  </threadedComment>
+  <threadedComment ref="F13" dT="2021-01-27T21:43:53.49" personId="{E59E69DB-0CAD-4A6E-A5B6-2A6254EA60D8}" id="{1869C771-C580-41CE-9D3C-793B204B87D5}">
+    <text>buy 4 packs of 8 pcs at GBP 3.99 each pack
+= total 32 pcs for 12 sets + extra</text>
+  </threadedComment>
+  <threadedComment ref="F19" dT="2021-01-27T21:40:23.79" personId="{E59E69DB-0CAD-4A6E-A5B6-2A6254EA60D8}" id="{58F8599A-228D-4E1E-90E9-143A66688545}">
+    <text>8 with the bolts, need 1 extra. Buy M3 nuts, 50pcs at GBP1.29 for 12 sets plus extra</text>
+  </threadedComment>
+  <threadedComment ref="F20" dT="2021-01-27T21:12:06.89" personId="{E59E69DB-0CAD-4A6E-A5B6-2A6254EA60D8}" id="{22C3FD05-C2BC-4ACA-B1F4-D6737862311B}">
+    <text>buy M3 x 6 with nuts, 2x 100pcs at GBP7.42 each = 200 pcs for 12 sets + extra</text>
+  </threadedComment>
+  <threadedComment ref="F21" dT="2021-01-27T21:04:27.32" personId="{E59E69DB-0CAD-4A6E-A5B6-2A6254EA60D8}" id="{88774207-C78B-40C9-8E79-3CBBD29570AA}">
+    <text>buy 100 pcs for GBP 6.85, for 12 sets + extra</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -680,7 +788,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,12 +835,12 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -743,39 +851,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E9469C-2C3E-4DDE-A657-7645A26DA7B8}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="81" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
       <c r="N1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -783,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -801,14 +911,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E12" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E23" si="0">C3*D3</f>
         <v>0</v>
       </c>
     </row>
@@ -817,7 +927,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -830,7 +940,7 @@
         <v>10.62</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -838,7 +948,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -854,7 +964,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -870,7 +980,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -886,31 +996,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
         <v>2.1</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>2.1</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -921,18 +1031,18 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
@@ -940,15 +1050,15 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -959,18 +1069,18 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
@@ -978,32 +1088,233 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
       <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D14" s="2" t="s">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="1">
-        <f>SUM(E2:E12)</f>
-        <v>28.319999999999997</v>
-      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
       <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
       <c r="D18" s="1"/>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7.4200000000000002E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.59360000000000002</v>
+      </c>
+      <c r="F20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="1">
+        <f>SUM(E2:E21)</f>
+        <v>27.087599999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D28" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>